<commit_message>
mcgill mapper runs! very slow though
</commit_message>
<xml_diff>
--- a/Data/Lab/McGill/mcgill_static.xlsx
+++ b/Data/Lab/McGill/mcgill_static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeandavidt/dev/jeandavidt/ODM Import/Data/Lab/McGill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867169DB-A5BD-7A45-A3CD-01CBF85F0991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76FE257-DF1F-8049-82E5-4C653B8084B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="500" windowWidth="19200" windowHeight="10560" tabRatio="806" activeTab="7" xr2:uid="{9CE44E43-4925-4F36-A354-815B16365F20}"/>
+    <workbookView xWindow="23200" yWindow="3640" windowWidth="20860" windowHeight="15300" tabRatio="806" firstSheet="6" activeTab="7" xr2:uid="{9CE44E43-4925-4F36-A354-815B16365F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="13" r:id="rId1"/>
@@ -2566,12 +2566,6 @@
     <t>PS_Gauze</t>
   </si>
   <si>
-    <t>Raw_Centrifuge</t>
-  </si>
-  <si>
-    <t>Raw_0.45um</t>
-  </si>
-  <si>
     <t>Raw_Centrifuge_0.45um</t>
   </si>
   <si>
@@ -2666,6 +2660,12 @@
   </si>
   <si>
     <t>frigon_lab_city_mtl</t>
+  </si>
+  <si>
+    <t>Raw_0.45um_alone</t>
+  </si>
+  <si>
+    <t>Raw_Centrifuge_alone</t>
   </si>
 </sst>
 </file>
@@ -3595,31 +3595,31 @@
     <xf numFmtId="171" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3649,49 +3649,31 @@
     <xf numFmtId="0" fontId="21" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3757,6 +3739,48 @@
     <xf numFmtId="0" fontId="22" fillId="13" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3791,30 +3815,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -13048,34 +13048,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="201" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="172"/>
-      <c r="L1" s="173"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="203"/>
     </row>
     <row r="2" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="176"/>
+      <c r="A2" s="204"/>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="205"/>
+      <c r="I2" s="205"/>
+      <c r="J2" s="205"/>
+      <c r="K2" s="205"/>
+      <c r="L2" s="206"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="162" t="s">
@@ -13122,50 +13122,50 @@
       <c r="L6" s="170"/>
     </row>
     <row r="7" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="153" t="s">
+      <c r="A7" s="174" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="154"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="159" t="s">
+      <c r="B7" s="175"/>
+      <c r="C7" s="175"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="175"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="171" t="s">
         <v>139</v>
       </c>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="160"/>
-      <c r="L7" s="161"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="172"/>
+      <c r="K7" s="172"/>
+      <c r="L7" s="173"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="153"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="154"/>
-      <c r="L8" s="155"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="175"/>
+      <c r="D8" s="175"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="175"/>
+      <c r="K8" s="175"/>
+      <c r="L8" s="176"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="156"/>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="158"/>
-      <c r="G9" s="156"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="157"/>
-      <c r="K9" s="157"/>
-      <c r="L9" s="158"/>
+      <c r="A9" s="177"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="178"/>
+      <c r="J9" s="178"/>
+      <c r="K9" s="178"/>
+      <c r="L9" s="179"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="162" t="s">
@@ -13212,50 +13212,50 @@
       <c r="L13" s="170"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="153" t="s">
+      <c r="A14" s="174" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="154"/>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="159" t="s">
+      <c r="B14" s="175"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="175"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="171" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
-      <c r="L14" s="161"/>
+      <c r="H14" s="172"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="172"/>
+      <c r="K14" s="172"/>
+      <c r="L14" s="173"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="153"/>
-      <c r="B15" s="154"/>
-      <c r="C15" s="154"/>
-      <c r="D15" s="154"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="155"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
-      <c r="L15" s="155"/>
+      <c r="A15" s="174"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="175"/>
+      <c r="F15" s="176"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="175"/>
+      <c r="I15" s="175"/>
+      <c r="J15" s="175"/>
+      <c r="K15" s="175"/>
+      <c r="L15" s="176"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="156"/>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="156"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="158"/>
+      <c r="A16" s="177"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="178"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="178"/>
+      <c r="L16" s="179"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="162" t="s">
@@ -13302,48 +13302,48 @@
       <c r="L21" s="170"/>
     </row>
     <row r="22" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="159" t="s">
+      <c r="A22" s="171" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="160"/>
-      <c r="C22" s="160"/>
-      <c r="D22" s="160"/>
-      <c r="E22" s="160"/>
-      <c r="F22" s="160"/>
-      <c r="G22" s="160"/>
-      <c r="H22" s="160"/>
-      <c r="I22" s="160"/>
-      <c r="J22" s="160"/>
-      <c r="K22" s="160"/>
-      <c r="L22" s="161"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="172"/>
+      <c r="I22" s="172"/>
+      <c r="J22" s="172"/>
+      <c r="K22" s="172"/>
+      <c r="L22" s="173"/>
     </row>
     <row r="23" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="153"/>
-      <c r="B23" s="154"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="154"/>
-      <c r="I23" s="154"/>
-      <c r="J23" s="154"/>
-      <c r="K23" s="154"/>
-      <c r="L23" s="155"/>
+      <c r="A23" s="174"/>
+      <c r="B23" s="175"/>
+      <c r="C23" s="175"/>
+      <c r="D23" s="175"/>
+      <c r="E23" s="175"/>
+      <c r="F23" s="175"/>
+      <c r="G23" s="175"/>
+      <c r="H23" s="175"/>
+      <c r="I23" s="175"/>
+      <c r="J23" s="175"/>
+      <c r="K23" s="175"/>
+      <c r="L23" s="176"/>
     </row>
     <row r="24" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="156"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="157"/>
-      <c r="L24" s="158"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="178"/>
+      <c r="C24" s="178"/>
+      <c r="D24" s="178"/>
+      <c r="E24" s="178"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="178"/>
+      <c r="J24" s="178"/>
+      <c r="K24" s="178"/>
+      <c r="L24" s="179"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="162" t="s">
@@ -13390,48 +13390,48 @@
       <c r="L29" s="170"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="159" t="s">
+      <c r="A30" s="171" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="160"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
-      <c r="H30" s="160"/>
-      <c r="I30" s="160"/>
-      <c r="J30" s="160"/>
-      <c r="K30" s="160"/>
-      <c r="L30" s="161"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
+      <c r="E30" s="172"/>
+      <c r="F30" s="172"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="172"/>
+      <c r="K30" s="172"/>
+      <c r="L30" s="173"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="153"/>
-      <c r="B31" s="154"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="154"/>
-      <c r="K31" s="154"/>
-      <c r="L31" s="155"/>
+      <c r="A31" s="174"/>
+      <c r="B31" s="175"/>
+      <c r="C31" s="175"/>
+      <c r="D31" s="175"/>
+      <c r="E31" s="175"/>
+      <c r="F31" s="175"/>
+      <c r="G31" s="175"/>
+      <c r="H31" s="175"/>
+      <c r="I31" s="175"/>
+      <c r="J31" s="175"/>
+      <c r="K31" s="175"/>
+      <c r="L31" s="176"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="156"/>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="157"/>
-      <c r="H32" s="157"/>
-      <c r="I32" s="157"/>
-      <c r="J32" s="157"/>
-      <c r="K32" s="157"/>
-      <c r="L32" s="158"/>
+      <c r="A32" s="177"/>
+      <c r="B32" s="178"/>
+      <c r="C32" s="178"/>
+      <c r="D32" s="178"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="178"/>
+      <c r="H32" s="178"/>
+      <c r="I32" s="178"/>
+      <c r="J32" s="178"/>
+      <c r="K32" s="178"/>
+      <c r="L32" s="179"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="162" t="s">
@@ -13478,83 +13478,76 @@
       <c r="L37" s="170"/>
     </row>
     <row r="38" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="186" t="s">
+      <c r="A38" s="180" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="187"/>
-      <c r="C38" s="187"/>
-      <c r="D38" s="187"/>
-      <c r="E38" s="192" t="s">
+      <c r="B38" s="181"/>
+      <c r="C38" s="181"/>
+      <c r="D38" s="181"/>
+      <c r="E38" s="186" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="193"/>
-      <c r="G38" s="193"/>
-      <c r="H38" s="193"/>
-      <c r="I38" s="198" t="s">
+      <c r="F38" s="187"/>
+      <c r="G38" s="187"/>
+      <c r="H38" s="187"/>
+      <c r="I38" s="192" t="s">
         <v>150</v>
       </c>
-      <c r="J38" s="199"/>
-      <c r="K38" s="199"/>
-      <c r="L38" s="200"/>
+      <c r="J38" s="193"/>
+      <c r="K38" s="193"/>
+      <c r="L38" s="194"/>
     </row>
     <row r="39" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="188"/>
-      <c r="B39" s="189"/>
-      <c r="C39" s="189"/>
-      <c r="D39" s="189"/>
-      <c r="E39" s="194"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="201"/>
-      <c r="J39" s="202"/>
-      <c r="K39" s="202"/>
-      <c r="L39" s="203"/>
+      <c r="A39" s="182"/>
+      <c r="B39" s="183"/>
+      <c r="C39" s="183"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="188"/>
+      <c r="F39" s="189"/>
+      <c r="G39" s="189"/>
+      <c r="H39" s="189"/>
+      <c r="I39" s="195"/>
+      <c r="J39" s="196"/>
+      <c r="K39" s="196"/>
+      <c r="L39" s="197"/>
     </row>
     <row r="40" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="190"/>
-      <c r="B40" s="191"/>
-      <c r="C40" s="191"/>
-      <c r="D40" s="191"/>
-      <c r="E40" s="196"/>
-      <c r="F40" s="197"/>
-      <c r="G40" s="197"/>
-      <c r="H40" s="197"/>
-      <c r="I40" s="204"/>
-      <c r="J40" s="205"/>
-      <c r="K40" s="205"/>
-      <c r="L40" s="206"/>
+      <c r="A40" s="184"/>
+      <c r="B40" s="185"/>
+      <c r="C40" s="185"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="190"/>
+      <c r="F40" s="191"/>
+      <c r="G40" s="191"/>
+      <c r="H40" s="191"/>
+      <c r="I40" s="198"/>
+      <c r="J40" s="199"/>
+      <c r="K40" s="199"/>
+      <c r="L40" s="200"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="153" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="178"/>
-      <c r="C41" s="178"/>
-      <c r="D41" s="179"/>
+      <c r="B41" s="154"/>
+      <c r="C41" s="154"/>
+      <c r="D41" s="155"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="180"/>
-      <c r="B42" s="181"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="182"/>
+      <c r="A42" s="156"/>
+      <c r="B42" s="157"/>
+      <c r="C42" s="157"/>
+      <c r="D42" s="158"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="183"/>
-      <c r="B43" s="184"/>
-      <c r="C43" s="184"/>
-      <c r="D43" s="185"/>
+      <c r="A43" s="159"/>
+      <c r="B43" s="160"/>
+      <c r="C43" s="160"/>
+      <c r="D43" s="161"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="YyYumUkpLd1R31zPFSpntUEyeBAjcNBny3cwqgmXYom4fFlL7EY0DaUXo1P0pgeoUSpryEqobBkdn+F+OVHbog==" saltValue="8pAW72rcGo8VyaZbMrEcGw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="16">
-    <mergeCell ref="A41:D43"/>
-    <mergeCell ref="A27:L29"/>
-    <mergeCell ref="A30:L32"/>
-    <mergeCell ref="A35:L37"/>
-    <mergeCell ref="A38:D40"/>
-    <mergeCell ref="E38:H40"/>
-    <mergeCell ref="I38:L40"/>
     <mergeCell ref="A14:F16"/>
     <mergeCell ref="G14:L16"/>
     <mergeCell ref="A19:L21"/>
@@ -13564,6 +13557,13 @@
     <mergeCell ref="A7:F9"/>
     <mergeCell ref="G7:L9"/>
     <mergeCell ref="A11:L13"/>
+    <mergeCell ref="A41:D43"/>
+    <mergeCell ref="A27:L29"/>
+    <mergeCell ref="A30:L32"/>
+    <mergeCell ref="A35:L37"/>
+    <mergeCell ref="A38:D40"/>
+    <mergeCell ref="E38:H40"/>
+    <mergeCell ref="I38:L40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A7:F9" location="Instrument!A1" display="Instrument" xr:uid="{68D40535-7CB1-438C-B5B4-17457BE8D8F6}"/>
@@ -13589,8 +13589,8 @@
   </sheetPr>
   <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="18.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13619,17 +13619,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="218" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="224" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="216"/>
+      <c r="C2" s="224"/>
       <c r="D2" s="136"/>
     </row>
     <row r="3" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="211"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="43" t="s">
         <v>0</v>
       </c>
@@ -13641,7 +13641,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="211"/>
+      <c r="A4" s="219"/>
       <c r="B4" s="43" t="s">
         <v>1</v>
       </c>
@@ -13653,7 +13653,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="211"/>
+      <c r="A5" s="219"/>
       <c r="B5" s="43" t="s">
         <v>2</v>
       </c>
@@ -13665,7 +13665,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="211"/>
+      <c r="A6" s="219"/>
       <c r="B6" s="43" t="s">
         <v>3</v>
       </c>
@@ -13677,7 +13677,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="211"/>
+      <c r="A7" s="219"/>
       <c r="B7" s="43" t="s">
         <v>4</v>
       </c>
@@ -13689,7 +13689,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="211"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="43" t="s">
         <v>5</v>
       </c>
@@ -13701,7 +13701,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="211"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="43" t="s">
         <v>6</v>
       </c>
@@ -13713,7 +13713,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="211"/>
+      <c r="A10" s="219"/>
       <c r="B10" s="43" t="s">
         <v>7</v>
       </c>
@@ -13725,7 +13725,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="211"/>
+      <c r="A11" s="219"/>
       <c r="B11" s="43" t="s">
         <v>8</v>
       </c>
@@ -13737,7 +13737,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="211"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="43" t="s">
         <v>9</v>
       </c>
@@ -13749,7 +13749,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="211"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="43" t="s">
         <v>170</v>
       </c>
@@ -13761,7 +13761,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="211"/>
+      <c r="A14" s="219"/>
       <c r="B14" s="43" t="s">
         <v>10</v>
       </c>
@@ -13773,7 +13773,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="211"/>
+      <c r="A15" s="219"/>
       <c r="B15" s="43" t="s">
         <v>11</v>
       </c>
@@ -13785,7 +13785,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="211"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="43" t="s">
         <v>175</v>
       </c>
@@ -13797,7 +13797,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="211"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="43" t="s">
         <v>13</v>
       </c>
@@ -13809,7 +13809,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="211"/>
+      <c r="A18" s="219"/>
       <c r="B18" s="43" t="s">
         <v>14</v>
       </c>
@@ -13821,7 +13821,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="211"/>
+      <c r="A19" s="219"/>
       <c r="B19" s="43" t="s">
         <v>15</v>
       </c>
@@ -13833,7 +13833,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="211"/>
+      <c r="A20" s="219"/>
       <c r="B20" s="43" t="s">
         <v>16</v>
       </c>
@@ -13845,7 +13845,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="211"/>
+      <c r="A21" s="219"/>
       <c r="B21" s="43" t="s">
         <v>17</v>
       </c>
@@ -13857,7 +13857,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="211"/>
+      <c r="A22" s="219"/>
       <c r="B22" s="43" t="s">
         <v>18</v>
       </c>
@@ -13869,7 +13869,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="212"/>
+      <c r="A23" s="220"/>
       <c r="B23" s="44" t="s">
         <v>19</v>
       </c>
@@ -13887,17 +13887,17 @@
       <c r="D25" s="130"/>
     </row>
     <row r="26" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="207" t="s">
+      <c r="A26" s="215" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="217" t="s">
+      <c r="B26" s="225" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="217"/>
+      <c r="C26" s="225"/>
       <c r="D26" s="137"/>
     </row>
     <row r="27" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="208"/>
+      <c r="A27" s="216"/>
       <c r="B27" s="43" t="s">
         <v>186</v>
       </c>
@@ -13910,7 +13910,7 @@
       <c r="E27"/>
     </row>
     <row r="28" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="208"/>
+      <c r="A28" s="216"/>
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
@@ -13923,7 +13923,7 @@
       <c r="E28"/>
     </row>
     <row r="29" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="208"/>
+      <c r="A29" s="216"/>
       <c r="B29" s="43" t="s">
         <v>24</v>
       </c>
@@ -13936,7 +13936,7 @@
       <c r="E29"/>
     </row>
     <row r="30" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="208"/>
+      <c r="A30" s="216"/>
       <c r="B30" s="43" t="s">
         <v>190</v>
       </c>
@@ -13949,7 +13949,7 @@
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="208"/>
+      <c r="A31" s="216"/>
       <c r="B31" s="43" t="s">
         <v>2</v>
       </c>
@@ -13962,7 +13962,7 @@
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="208"/>
+      <c r="A32" s="216"/>
       <c r="B32" s="43" t="s">
         <v>3</v>
       </c>
@@ -13975,7 +13975,7 @@
       <c r="E32"/>
     </row>
     <row r="33" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="208"/>
+      <c r="A33" s="216"/>
       <c r="B33" s="43" t="s">
         <v>26</v>
       </c>
@@ -13988,7 +13988,7 @@
       <c r="E33"/>
     </row>
     <row r="34" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="208"/>
+      <c r="A34" s="216"/>
       <c r="B34" s="43" t="s">
         <v>27</v>
       </c>
@@ -14001,7 +14001,7 @@
       <c r="E34"/>
     </row>
     <row r="35" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="208"/>
+      <c r="A35" s="216"/>
       <c r="B35" s="43" t="s">
         <v>28</v>
       </c>
@@ -14014,7 +14014,7 @@
       <c r="E35"/>
     </row>
     <row r="36" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="208"/>
+      <c r="A36" s="216"/>
       <c r="B36" s="43" t="s">
         <v>7</v>
       </c>
@@ -14027,7 +14027,7 @@
       <c r="E36"/>
     </row>
     <row r="37" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="208"/>
+      <c r="A37" s="216"/>
       <c r="B37" s="43" t="s">
         <v>30</v>
       </c>
@@ -14040,7 +14040,7 @@
       <c r="E37"/>
     </row>
     <row r="38" spans="1:10" s="18" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="208"/>
+      <c r="A38" s="216"/>
       <c r="B38" s="43" t="s">
         <v>31</v>
       </c>
@@ -14053,7 +14053,7 @@
       <c r="E38"/>
     </row>
     <row r="39" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="208"/>
+      <c r="A39" s="216"/>
       <c r="B39" s="43" t="s">
         <v>14</v>
       </c>
@@ -14066,7 +14066,7 @@
       <c r="E39"/>
     </row>
     <row r="40" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="208"/>
+      <c r="A40" s="216"/>
       <c r="B40" s="43" t="s">
         <v>29</v>
       </c>
@@ -14079,7 +14079,7 @@
       <c r="E40"/>
     </row>
     <row r="41" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="208"/>
+      <c r="A41" s="216"/>
       <c r="B41" s="43" t="s">
         <v>18</v>
       </c>
@@ -14092,7 +14092,7 @@
       <c r="E41"/>
     </row>
     <row r="42" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="208"/>
+      <c r="A42" s="216"/>
       <c r="B42" s="43" t="s">
         <v>32</v>
       </c>
@@ -14105,7 +14105,7 @@
       <c r="E42"/>
     </row>
     <row r="43" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="208"/>
+      <c r="A43" s="216"/>
       <c r="B43" s="43" t="s">
         <v>33</v>
       </c>
@@ -14118,7 +14118,7 @@
       <c r="E43"/>
     </row>
     <row r="44" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="208"/>
+      <c r="A44" s="216"/>
       <c r="B44" s="43" t="s">
         <v>34</v>
       </c>
@@ -14135,7 +14135,7 @@
       <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="208"/>
+      <c r="A45" s="216"/>
       <c r="B45" s="43" t="s">
         <v>35</v>
       </c>
@@ -14148,7 +14148,7 @@
       <c r="E45"/>
     </row>
     <row r="46" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="208"/>
+      <c r="A46" s="216"/>
       <c r="B46" s="43" t="s">
         <v>36</v>
       </c>
@@ -14161,7 +14161,7 @@
       <c r="E46"/>
     </row>
     <row r="47" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="208"/>
+      <c r="A47" s="216"/>
       <c r="B47" s="43" t="s">
         <v>37</v>
       </c>
@@ -14174,7 +14174,7 @@
       <c r="E47"/>
     </row>
     <row r="48" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="208"/>
+      <c r="A48" s="216"/>
       <c r="B48" s="43" t="s">
         <v>38</v>
       </c>
@@ -14187,7 +14187,7 @@
       <c r="E48"/>
     </row>
     <row r="49" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="209"/>
+      <c r="A49" s="217"/>
       <c r="B49" s="44" t="s">
         <v>19</v>
       </c>
@@ -14210,18 +14210,18 @@
       <c r="E51"/>
     </row>
     <row r="52" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="213" t="s">
+      <c r="A52" s="221" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="218" t="s">
+      <c r="B52" s="226" t="s">
         <v>210</v>
       </c>
-      <c r="C52" s="218"/>
+      <c r="C52" s="226"/>
       <c r="D52" s="138"/>
       <c r="E52"/>
     </row>
     <row r="53" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="214"/>
+      <c r="A53" s="222"/>
       <c r="B53" s="43" t="s">
         <v>54</v>
       </c>
@@ -14235,7 +14235,7 @@
       <c r="F53" s="131"/>
     </row>
     <row r="54" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="214"/>
+      <c r="A54" s="222"/>
       <c r="B54" s="43" t="s">
         <v>1</v>
       </c>
@@ -14249,7 +14249,7 @@
       <c r="F54" s="131"/>
     </row>
     <row r="55" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="214"/>
+      <c r="A55" s="222"/>
       <c r="B55" s="43" t="s">
         <v>2</v>
       </c>
@@ -14263,7 +14263,7 @@
       <c r="F55" s="131"/>
     </row>
     <row r="56" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="214"/>
+      <c r="A56" s="222"/>
       <c r="B56" s="43" t="s">
         <v>0</v>
       </c>
@@ -14277,7 +14277,7 @@
       <c r="F56" s="131"/>
     </row>
     <row r="57" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="214"/>
+      <c r="A57" s="222"/>
       <c r="B57" s="43" t="s">
         <v>3</v>
       </c>
@@ -14291,7 +14291,7 @@
       <c r="F57" s="131"/>
     </row>
     <row r="58" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="214"/>
+      <c r="A58" s="222"/>
       <c r="B58" s="43" t="s">
         <v>4</v>
       </c>
@@ -14305,7 +14305,7 @@
       <c r="F58" s="131"/>
     </row>
     <row r="59" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="214"/>
+      <c r="A59" s="222"/>
       <c r="B59" s="43" t="s">
         <v>7</v>
       </c>
@@ -14319,7 +14319,7 @@
       <c r="F59" s="131"/>
     </row>
     <row r="60" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="214"/>
+      <c r="A60" s="222"/>
       <c r="B60" s="43" t="s">
         <v>31</v>
       </c>
@@ -14333,7 +14333,7 @@
       <c r="F60" s="131"/>
     </row>
     <row r="61" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="214"/>
+      <c r="A61" s="222"/>
       <c r="B61" s="43" t="s">
         <v>55</v>
       </c>
@@ -14347,7 +14347,7 @@
       <c r="F61" s="131"/>
     </row>
     <row r="62" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="214"/>
+      <c r="A62" s="222"/>
       <c r="B62" s="43" t="s">
         <v>29</v>
       </c>
@@ -14361,7 +14361,7 @@
       <c r="F62" s="131"/>
     </row>
     <row r="63" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="214"/>
+      <c r="A63" s="222"/>
       <c r="B63" s="43" t="s">
         <v>30</v>
       </c>
@@ -14375,7 +14375,7 @@
       <c r="F63" s="131"/>
     </row>
     <row r="64" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="214"/>
+      <c r="A64" s="222"/>
       <c r="B64" s="43" t="s">
         <v>18</v>
       </c>
@@ -14389,7 +14389,7 @@
       <c r="F64" s="131"/>
     </row>
     <row r="65" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="214"/>
+      <c r="A65" s="222"/>
       <c r="B65" s="43" t="s">
         <v>32</v>
       </c>
@@ -14403,7 +14403,7 @@
       <c r="F65" s="131"/>
     </row>
     <row r="66" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="214"/>
+      <c r="A66" s="222"/>
       <c r="B66" s="43" t="s">
         <v>33</v>
       </c>
@@ -14417,7 +14417,7 @@
       <c r="F66" s="131"/>
     </row>
     <row r="67" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="214"/>
+      <c r="A67" s="222"/>
       <c r="B67" s="43" t="s">
         <v>34</v>
       </c>
@@ -14431,7 +14431,7 @@
       <c r="F67" s="131"/>
     </row>
     <row r="68" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="214"/>
+      <c r="A68" s="222"/>
       <c r="B68" s="43" t="s">
         <v>35</v>
       </c>
@@ -14445,7 +14445,7 @@
       <c r="F68" s="131"/>
     </row>
     <row r="69" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="214"/>
+      <c r="A69" s="222"/>
       <c r="B69" s="43" t="s">
         <v>36</v>
       </c>
@@ -14459,7 +14459,7 @@
       <c r="F69" s="131"/>
     </row>
     <row r="70" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="214"/>
+      <c r="A70" s="222"/>
       <c r="B70" s="43" t="s">
         <v>37</v>
       </c>
@@ -14473,7 +14473,7 @@
       <c r="F70" s="131"/>
     </row>
     <row r="71" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="214"/>
+      <c r="A71" s="222"/>
       <c r="B71" s="43" t="s">
         <v>38</v>
       </c>
@@ -14487,7 +14487,7 @@
       <c r="F71" s="131"/>
     </row>
     <row r="72" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="215"/>
+      <c r="A72" s="223"/>
       <c r="B72" s="44" t="s">
         <v>19</v>
       </c>
@@ -14517,19 +14517,19 @@
       <c r="F74" s="131"/>
     </row>
     <row r="75" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="219" t="s">
+      <c r="A75" s="211" t="s">
         <v>224</v>
       </c>
-      <c r="B75" s="225" t="s">
+      <c r="B75" s="214" t="s">
         <v>225</v>
       </c>
-      <c r="C75" s="225"/>
+      <c r="C75" s="214"/>
       <c r="D75" s="139"/>
       <c r="E75"/>
       <c r="F75" s="131"/>
     </row>
     <row r="76" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="220"/>
+      <c r="A76" s="212"/>
       <c r="B76" s="43" t="s">
         <v>70</v>
       </c>
@@ -14542,7 +14542,7 @@
       <c r="F76" s="131"/>
     </row>
     <row r="77" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="220"/>
+      <c r="A77" s="212"/>
       <c r="B77" s="43" t="s">
         <v>3</v>
       </c>
@@ -14554,7 +14554,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="220"/>
+      <c r="A78" s="212"/>
       <c r="B78" s="43" t="s">
         <v>71</v>
       </c>
@@ -14566,7 +14566,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="220"/>
+      <c r="A79" s="212"/>
       <c r="B79" s="43" t="s">
         <v>72</v>
       </c>
@@ -14578,7 +14578,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="220"/>
+      <c r="A80" s="212"/>
       <c r="B80" s="43" t="s">
         <v>7</v>
       </c>
@@ -14590,7 +14590,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="220"/>
+      <c r="A81" s="212"/>
       <c r="B81" s="43" t="s">
         <v>73</v>
       </c>
@@ -14602,7 +14602,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="220"/>
+      <c r="A82" s="212"/>
       <c r="B82" s="43" t="s">
         <v>29</v>
       </c>
@@ -14614,7 +14614,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="221"/>
+      <c r="A83" s="213"/>
       <c r="B83" s="44" t="s">
         <v>19</v>
       </c>
@@ -14627,17 +14627,17 @@
     </row>
     <row r="84" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="86" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="222" t="s">
+      <c r="A86" s="207" t="s">
         <v>142</v>
       </c>
-      <c r="B86" s="226" t="s">
+      <c r="B86" s="210" t="s">
         <v>233</v>
       </c>
-      <c r="C86" s="226"/>
+      <c r="C86" s="210"/>
       <c r="D86" s="140"/>
     </row>
     <row r="87" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="223"/>
+      <c r="A87" s="208"/>
       <c r="B87" s="43" t="s">
         <v>25</v>
       </c>
@@ -14649,7 +14649,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="223"/>
+      <c r="A88" s="208"/>
       <c r="B88" s="43" t="s">
         <v>2</v>
       </c>
@@ -14661,7 +14661,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="223"/>
+      <c r="A89" s="208"/>
       <c r="B89" s="43" t="s">
         <v>80</v>
       </c>
@@ -14673,7 +14673,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="223"/>
+      <c r="A90" s="208"/>
       <c r="B90" s="43" t="s">
         <v>100</v>
       </c>
@@ -14685,7 +14685,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="223"/>
+      <c r="A91" s="208"/>
       <c r="B91" s="43" t="s">
         <v>101</v>
       </c>
@@ -14697,7 +14697,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="223"/>
+      <c r="A92" s="208"/>
       <c r="B92" s="43" t="s">
         <v>91</v>
       </c>
@@ -14709,7 +14709,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="223"/>
+      <c r="A93" s="208"/>
       <c r="B93" s="43" t="s">
         <v>72</v>
       </c>
@@ -14721,7 +14721,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="223"/>
+      <c r="A94" s="208"/>
       <c r="B94" s="43" t="s">
         <v>102</v>
       </c>
@@ -14733,7 +14733,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="223"/>
+      <c r="A95" s="208"/>
       <c r="B95" s="43" t="s">
         <v>104</v>
       </c>
@@ -14745,7 +14745,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="223"/>
+      <c r="A96" s="208"/>
       <c r="B96" s="43" t="s">
         <v>103</v>
       </c>
@@ -14757,7 +14757,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="223"/>
+      <c r="A97" s="208"/>
       <c r="B97" s="43" t="s">
         <v>30</v>
       </c>
@@ -14769,7 +14769,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="223"/>
+      <c r="A98" s="208"/>
       <c r="B98" s="43" t="s">
         <v>105</v>
       </c>
@@ -14781,7 +14781,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="223"/>
+      <c r="A99" s="208"/>
       <c r="B99" s="43" t="s">
         <v>246</v>
       </c>
@@ -14793,7 +14793,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="223"/>
+      <c r="A100" s="208"/>
       <c r="B100" s="43" t="s">
         <v>248</v>
       </c>
@@ -14805,7 +14805,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="223"/>
+      <c r="A101" s="208"/>
       <c r="B101" s="43" t="s">
         <v>108</v>
       </c>
@@ -14817,7 +14817,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="223"/>
+      <c r="A102" s="208"/>
       <c r="B102" s="43" t="s">
         <v>109</v>
       </c>
@@ -14829,7 +14829,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="223"/>
+      <c r="A103" s="208"/>
       <c r="B103" s="43" t="s">
         <v>110</v>
       </c>
@@ -14841,7 +14841,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="224"/>
+      <c r="A104" s="209"/>
       <c r="B104" s="44" t="s">
         <v>19</v>
       </c>
@@ -14853,17 +14853,17 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="222" t="s">
+      <c r="A107" s="207" t="s">
         <v>141</v>
       </c>
-      <c r="B107" s="226" t="s">
+      <c r="B107" s="210" t="s">
         <v>253</v>
       </c>
-      <c r="C107" s="226"/>
+      <c r="C107" s="210"/>
       <c r="D107" s="140"/>
     </row>
     <row r="108" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="223"/>
+      <c r="A108" s="208"/>
       <c r="B108" s="43" t="s">
         <v>1</v>
       </c>
@@ -14875,7 +14875,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="223"/>
+      <c r="A109" s="208"/>
       <c r="B109" s="43" t="s">
         <v>80</v>
       </c>
@@ -14887,7 +14887,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="223"/>
+      <c r="A110" s="208"/>
       <c r="B110" s="43" t="s">
         <v>86</v>
       </c>
@@ -14899,7 +14899,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="223"/>
+      <c r="A111" s="208"/>
       <c r="B111" s="43" t="s">
         <v>87</v>
       </c>
@@ -14911,7 +14911,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="223"/>
+      <c r="A112" s="208"/>
       <c r="B112" s="43" t="s">
         <v>88</v>
       </c>
@@ -14923,7 +14923,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="223"/>
+      <c r="A113" s="208"/>
       <c r="B113" s="43" t="s">
         <v>7</v>
       </c>
@@ -14935,7 +14935,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="223"/>
+      <c r="A114" s="208"/>
       <c r="B114" s="43" t="s">
         <v>89</v>
       </c>
@@ -14947,7 +14947,7 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="223"/>
+      <c r="A115" s="208"/>
       <c r="B115" s="43" t="s">
         <v>90</v>
       </c>
@@ -14959,7 +14959,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="223"/>
+      <c r="A116" s="208"/>
       <c r="B116" s="43" t="s">
         <v>71</v>
       </c>
@@ -14972,7 +14972,7 @@
       <c r="E116" s="135"/>
     </row>
     <row r="117" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="223"/>
+      <c r="A117" s="208"/>
       <c r="B117" s="43" t="s">
         <v>91</v>
       </c>
@@ -14985,7 +14985,7 @@
       <c r="E117" s="135"/>
     </row>
     <row r="118" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="224"/>
+      <c r="A118" s="209"/>
       <c r="B118" s="44" t="s">
         <v>19</v>
       </c>
@@ -14997,17 +14997,17 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="222" t="s">
+      <c r="A121" s="207" t="s">
         <v>144</v>
       </c>
-      <c r="B121" s="226" t="s">
+      <c r="B121" s="210" t="s">
         <v>264</v>
       </c>
-      <c r="C121" s="226"/>
+      <c r="C121" s="210"/>
       <c r="D121" s="140"/>
     </row>
     <row r="122" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="223"/>
+      <c r="A122" s="208"/>
       <c r="B122" s="43" t="s">
         <v>24</v>
       </c>
@@ -15019,7 +15019,7 @@
       </c>
     </row>
     <row r="123" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="223"/>
+      <c r="A123" s="208"/>
       <c r="B123" s="43" t="s">
         <v>80</v>
       </c>
@@ -15031,7 +15031,7 @@
       </c>
     </row>
     <row r="124" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="223"/>
+      <c r="A124" s="208"/>
       <c r="B124" s="43" t="s">
         <v>74</v>
       </c>
@@ -15043,7 +15043,7 @@
       </c>
     </row>
     <row r="125" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="223"/>
+      <c r="A125" s="208"/>
       <c r="B125" s="43" t="s">
         <v>75</v>
       </c>
@@ -15055,7 +15055,7 @@
       </c>
     </row>
     <row r="126" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="223"/>
+      <c r="A126" s="208"/>
       <c r="B126" s="43" t="s">
         <v>77</v>
       </c>
@@ -15067,7 +15067,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="223"/>
+      <c r="A127" s="208"/>
       <c r="B127" s="43" t="s">
         <v>270</v>
       </c>
@@ -15079,7 +15079,7 @@
       </c>
     </row>
     <row r="128" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="224"/>
+      <c r="A128" s="209"/>
       <c r="B128" s="44" t="s">
         <v>19</v>
       </c>
@@ -15091,17 +15091,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="222" t="s">
+      <c r="A131" s="207" t="s">
         <v>138</v>
       </c>
-      <c r="B131" s="226" t="s">
+      <c r="B131" s="210" t="s">
         <v>272</v>
       </c>
-      <c r="C131" s="226"/>
+      <c r="C131" s="210"/>
       <c r="D131" s="140"/>
     </row>
     <row r="132" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="223"/>
+      <c r="A132" s="208"/>
       <c r="B132" s="43" t="s">
         <v>2</v>
       </c>
@@ -15113,7 +15113,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="223"/>
+      <c r="A133" s="208"/>
       <c r="B133" s="43" t="s">
         <v>80</v>
       </c>
@@ -15125,7 +15125,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="223"/>
+      <c r="A134" s="208"/>
       <c r="B134" s="43" t="s">
         <v>115</v>
       </c>
@@ -15137,7 +15137,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="223"/>
+      <c r="A135" s="208"/>
       <c r="B135" s="43" t="s">
         <v>276</v>
       </c>
@@ -15149,7 +15149,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="223"/>
+      <c r="A136" s="208"/>
       <c r="B136" s="43" t="s">
         <v>116</v>
       </c>
@@ -15161,7 +15161,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="223"/>
+      <c r="A137" s="208"/>
       <c r="B137" s="43" t="s">
         <v>7</v>
       </c>
@@ -15173,7 +15173,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="224"/>
+      <c r="A138" s="209"/>
       <c r="B138" s="44" t="s">
         <v>19</v>
       </c>
@@ -15191,17 +15191,17 @@
       <c r="C140" s="112"/>
     </row>
     <row r="141" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="222" t="s">
+      <c r="A141" s="207" t="s">
         <v>146</v>
       </c>
-      <c r="B141" s="226" t="s">
+      <c r="B141" s="210" t="s">
         <v>280</v>
       </c>
-      <c r="C141" s="226"/>
+      <c r="C141" s="210"/>
       <c r="D141" s="140"/>
     </row>
     <row r="142" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="223"/>
+      <c r="A142" s="208"/>
       <c r="B142" s="43" t="s">
         <v>3</v>
       </c>
@@ -15213,7 +15213,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="223"/>
+      <c r="A143" s="208"/>
       <c r="B143" s="43" t="s">
         <v>74</v>
       </c>
@@ -15225,7 +15225,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="223"/>
+      <c r="A144" s="208"/>
       <c r="B144" s="43" t="s">
         <v>75</v>
       </c>
@@ -15237,7 +15237,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="223"/>
+      <c r="A145" s="208"/>
       <c r="B145" s="43" t="s">
         <v>284</v>
       </c>
@@ -15249,7 +15249,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="223"/>
+      <c r="A146" s="208"/>
       <c r="B146" s="43" t="s">
         <v>77</v>
       </c>
@@ -15261,7 +15261,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="224"/>
+      <c r="A147" s="209"/>
       <c r="B147" s="44" t="s">
         <v>19</v>
       </c>
@@ -15273,17 +15273,17 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="222" t="s">
+      <c r="A150" s="207" t="s">
         <v>139</v>
       </c>
-      <c r="B150" s="226" t="s">
+      <c r="B150" s="210" t="s">
         <v>287</v>
       </c>
-      <c r="C150" s="226"/>
+      <c r="C150" s="210"/>
       <c r="D150" s="140"/>
     </row>
     <row r="151" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="223"/>
+      <c r="A151" s="208"/>
       <c r="B151" s="43" t="s">
         <v>71</v>
       </c>
@@ -15295,7 +15295,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="223"/>
+      <c r="A152" s="208"/>
       <c r="B152" s="43" t="s">
         <v>80</v>
       </c>
@@ -15307,7 +15307,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="223"/>
+      <c r="A153" s="208"/>
       <c r="B153" s="43" t="s">
         <v>126</v>
       </c>
@@ -15319,7 +15319,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="223"/>
+      <c r="A154" s="208"/>
       <c r="B154" s="43" t="s">
         <v>7</v>
       </c>
@@ -15331,7 +15331,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="223"/>
+      <c r="A155" s="208"/>
       <c r="B155" s="43" t="s">
         <v>127</v>
       </c>
@@ -15343,7 +15343,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="223"/>
+      <c r="A156" s="208"/>
       <c r="B156" s="43" t="s">
         <v>91</v>
       </c>
@@ -15355,7 +15355,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="224"/>
+      <c r="A157" s="209"/>
       <c r="B157" s="44" t="s">
         <v>19</v>
       </c>
@@ -15368,6 +15368,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="A52:A72"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A75:A83"/>
+    <mergeCell ref="A86:A104"/>
+    <mergeCell ref="A107:A118"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B86:C86"/>
     <mergeCell ref="A150:A157"/>
     <mergeCell ref="A121:A128"/>
     <mergeCell ref="A131:A138"/>
@@ -15376,18 +15388,6 @@
     <mergeCell ref="B131:C131"/>
     <mergeCell ref="B141:C141"/>
     <mergeCell ref="B150:C150"/>
-    <mergeCell ref="A75:A83"/>
-    <mergeCell ref="A86:A104"/>
-    <mergeCell ref="A107:A118"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A52:A72"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B90" r:id="rId1" display="https://semver.org/" xr:uid="{E5C4F3F2-C2D3-41B6-ABD9-C7AEBA6C45F1}"/>
@@ -16882,34 +16882,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="201" t="s">
         <v>525</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="172"/>
-      <c r="J1" s="172"/>
-      <c r="K1" s="172"/>
-      <c r="L1" s="173"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="203"/>
     </row>
     <row r="2" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="174"/>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="176"/>
+      <c r="A2" s="204"/>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="205"/>
+      <c r="I2" s="205"/>
+      <c r="J2" s="205"/>
+      <c r="K2" s="205"/>
+      <c r="L2" s="206"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="162" t="s">
@@ -16956,50 +16956,50 @@
       <c r="L6" s="170"/>
     </row>
     <row r="7" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="153" t="s">
+      <c r="A7" s="174" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="154"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="159" t="s">
+      <c r="B7" s="175"/>
+      <c r="C7" s="175"/>
+      <c r="D7" s="175"/>
+      <c r="E7" s="175"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="171" t="s">
         <v>139</v>
       </c>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="160"/>
-      <c r="L7" s="161"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="172"/>
+      <c r="K7" s="172"/>
+      <c r="L7" s="173"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="153"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="153"/>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="154"/>
-      <c r="L8" s="155"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="175"/>
+      <c r="D8" s="175"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="175"/>
+      <c r="K8" s="175"/>
+      <c r="L8" s="176"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="156"/>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="158"/>
-      <c r="G9" s="156"/>
-      <c r="H9" s="157"/>
-      <c r="I9" s="157"/>
-      <c r="J9" s="157"/>
-      <c r="K9" s="157"/>
-      <c r="L9" s="158"/>
+      <c r="A9" s="177"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="178"/>
+      <c r="J9" s="178"/>
+      <c r="K9" s="178"/>
+      <c r="L9" s="179"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="162" t="s">
@@ -17046,50 +17046,50 @@
       <c r="L13" s="170"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="153" t="s">
+      <c r="A14" s="174" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="154"/>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="155"/>
-      <c r="G14" s="159" t="s">
+      <c r="B14" s="175"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="175"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="171" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
-      <c r="L14" s="161"/>
+      <c r="H14" s="172"/>
+      <c r="I14" s="172"/>
+      <c r="J14" s="172"/>
+      <c r="K14" s="172"/>
+      <c r="L14" s="173"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="153"/>
-      <c r="B15" s="154"/>
-      <c r="C15" s="154"/>
-      <c r="D15" s="154"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="155"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
-      <c r="L15" s="155"/>
+      <c r="A15" s="174"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="175"/>
+      <c r="F15" s="176"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="175"/>
+      <c r="I15" s="175"/>
+      <c r="J15" s="175"/>
+      <c r="K15" s="175"/>
+      <c r="L15" s="176"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="156"/>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="156"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="158"/>
+      <c r="A16" s="177"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="178"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="178"/>
+      <c r="L16" s="179"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="162" t="s">
@@ -17136,48 +17136,48 @@
       <c r="L21" s="170"/>
     </row>
     <row r="22" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="159" t="s">
+      <c r="A22" s="171" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="160"/>
-      <c r="C22" s="160"/>
-      <c r="D22" s="160"/>
-      <c r="E22" s="160"/>
-      <c r="F22" s="160"/>
-      <c r="G22" s="160"/>
-      <c r="H22" s="160"/>
-      <c r="I22" s="160"/>
-      <c r="J22" s="160"/>
-      <c r="K22" s="160"/>
-      <c r="L22" s="161"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="172"/>
+      <c r="I22" s="172"/>
+      <c r="J22" s="172"/>
+      <c r="K22" s="172"/>
+      <c r="L22" s="173"/>
     </row>
     <row r="23" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="153"/>
-      <c r="B23" s="154"/>
-      <c r="C23" s="154"/>
-      <c r="D23" s="154"/>
-      <c r="E23" s="154"/>
-      <c r="F23" s="154"/>
-      <c r="G23" s="154"/>
-      <c r="H23" s="154"/>
-      <c r="I23" s="154"/>
-      <c r="J23" s="154"/>
-      <c r="K23" s="154"/>
-      <c r="L23" s="155"/>
+      <c r="A23" s="174"/>
+      <c r="B23" s="175"/>
+      <c r="C23" s="175"/>
+      <c r="D23" s="175"/>
+      <c r="E23" s="175"/>
+      <c r="F23" s="175"/>
+      <c r="G23" s="175"/>
+      <c r="H23" s="175"/>
+      <c r="I23" s="175"/>
+      <c r="J23" s="175"/>
+      <c r="K23" s="175"/>
+      <c r="L23" s="176"/>
     </row>
     <row r="24" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="156"/>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="157"/>
-      <c r="L24" s="158"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="178"/>
+      <c r="C24" s="178"/>
+      <c r="D24" s="178"/>
+      <c r="E24" s="178"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="178"/>
+      <c r="J24" s="178"/>
+      <c r="K24" s="178"/>
+      <c r="L24" s="179"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="162" t="s">
@@ -17224,48 +17224,48 @@
       <c r="L29" s="170"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="159" t="s">
+      <c r="A30" s="171" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="160"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160"/>
-      <c r="H30" s="160"/>
-      <c r="I30" s="160"/>
-      <c r="J30" s="160"/>
-      <c r="K30" s="160"/>
-      <c r="L30" s="161"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="172"/>
+      <c r="D30" s="172"/>
+      <c r="E30" s="172"/>
+      <c r="F30" s="172"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="172"/>
+      <c r="J30" s="172"/>
+      <c r="K30" s="172"/>
+      <c r="L30" s="173"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="153"/>
-      <c r="B31" s="154"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="154"/>
-      <c r="K31" s="154"/>
-      <c r="L31" s="155"/>
+      <c r="A31" s="174"/>
+      <c r="B31" s="175"/>
+      <c r="C31" s="175"/>
+      <c r="D31" s="175"/>
+      <c r="E31" s="175"/>
+      <c r="F31" s="175"/>
+      <c r="G31" s="175"/>
+      <c r="H31" s="175"/>
+      <c r="I31" s="175"/>
+      <c r="J31" s="175"/>
+      <c r="K31" s="175"/>
+      <c r="L31" s="176"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="156"/>
-      <c r="B32" s="157"/>
-      <c r="C32" s="157"/>
-      <c r="D32" s="157"/>
-      <c r="E32" s="157"/>
-      <c r="F32" s="157"/>
-      <c r="G32" s="157"/>
-      <c r="H32" s="157"/>
-      <c r="I32" s="157"/>
-      <c r="J32" s="157"/>
-      <c r="K32" s="157"/>
-      <c r="L32" s="158"/>
+      <c r="A32" s="177"/>
+      <c r="B32" s="178"/>
+      <c r="C32" s="178"/>
+      <c r="D32" s="178"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="178"/>
+      <c r="H32" s="178"/>
+      <c r="I32" s="178"/>
+      <c r="J32" s="178"/>
+      <c r="K32" s="178"/>
+      <c r="L32" s="179"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="162" t="s">
@@ -17312,75 +17312,82 @@
       <c r="L37" s="170"/>
     </row>
     <row r="38" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="186" t="s">
+      <c r="A38" s="180" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="187"/>
-      <c r="C38" s="187"/>
-      <c r="D38" s="187"/>
-      <c r="E38" s="192" t="s">
+      <c r="B38" s="181"/>
+      <c r="C38" s="181"/>
+      <c r="D38" s="181"/>
+      <c r="E38" s="186" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="193"/>
-      <c r="G38" s="193"/>
-      <c r="H38" s="193"/>
-      <c r="I38" s="198" t="s">
+      <c r="F38" s="187"/>
+      <c r="G38" s="187"/>
+      <c r="H38" s="187"/>
+      <c r="I38" s="192" t="s">
         <v>150</v>
       </c>
-      <c r="J38" s="199"/>
-      <c r="K38" s="199"/>
-      <c r="L38" s="200"/>
+      <c r="J38" s="193"/>
+      <c r="K38" s="193"/>
+      <c r="L38" s="194"/>
     </row>
     <row r="39" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="188"/>
-      <c r="B39" s="189"/>
-      <c r="C39" s="189"/>
-      <c r="D39" s="189"/>
-      <c r="E39" s="194"/>
-      <c r="F39" s="195"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="195"/>
-      <c r="I39" s="201"/>
-      <c r="J39" s="202"/>
-      <c r="K39" s="202"/>
-      <c r="L39" s="203"/>
+      <c r="A39" s="182"/>
+      <c r="B39" s="183"/>
+      <c r="C39" s="183"/>
+      <c r="D39" s="183"/>
+      <c r="E39" s="188"/>
+      <c r="F39" s="189"/>
+      <c r="G39" s="189"/>
+      <c r="H39" s="189"/>
+      <c r="I39" s="195"/>
+      <c r="J39" s="196"/>
+      <c r="K39" s="196"/>
+      <c r="L39" s="197"/>
     </row>
     <row r="40" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="190"/>
-      <c r="B40" s="191"/>
-      <c r="C40" s="191"/>
-      <c r="D40" s="191"/>
-      <c r="E40" s="196"/>
-      <c r="F40" s="197"/>
-      <c r="G40" s="197"/>
-      <c r="H40" s="197"/>
-      <c r="I40" s="204"/>
-      <c r="J40" s="205"/>
-      <c r="K40" s="205"/>
-      <c r="L40" s="206"/>
+      <c r="A40" s="184"/>
+      <c r="B40" s="185"/>
+      <c r="C40" s="185"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="190"/>
+      <c r="F40" s="191"/>
+      <c r="G40" s="191"/>
+      <c r="H40" s="191"/>
+      <c r="I40" s="198"/>
+      <c r="J40" s="199"/>
+      <c r="K40" s="199"/>
+      <c r="L40" s="200"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="177" t="s">
+      <c r="A41" s="153" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="178"/>
-      <c r="C41" s="178"/>
-      <c r="D41" s="179"/>
+      <c r="B41" s="154"/>
+      <c r="C41" s="154"/>
+      <c r="D41" s="155"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="180"/>
-      <c r="B42" s="181"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="182"/>
+      <c r="A42" s="156"/>
+      <c r="B42" s="157"/>
+      <c r="C42" s="157"/>
+      <c r="D42" s="158"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="183"/>
-      <c r="B43" s="184"/>
-      <c r="C43" s="184"/>
-      <c r="D43" s="185"/>
+      <c r="A43" s="159"/>
+      <c r="B43" s="160"/>
+      <c r="C43" s="160"/>
+      <c r="D43" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A14:F16"/>
+    <mergeCell ref="G14:L16"/>
+    <mergeCell ref="A1:L2"/>
+    <mergeCell ref="A4:L6"/>
+    <mergeCell ref="A7:F9"/>
+    <mergeCell ref="G7:L9"/>
+    <mergeCell ref="A11:L13"/>
     <mergeCell ref="A41:D43"/>
     <mergeCell ref="A19:L21"/>
     <mergeCell ref="A22:L24"/>
@@ -17390,13 +17397,6 @@
     <mergeCell ref="A38:D40"/>
     <mergeCell ref="E38:H40"/>
     <mergeCell ref="I38:L40"/>
-    <mergeCell ref="A14:F16"/>
-    <mergeCell ref="G14:L16"/>
-    <mergeCell ref="A1:L2"/>
-    <mergeCell ref="A4:L6"/>
-    <mergeCell ref="A7:F9"/>
-    <mergeCell ref="G7:L9"/>
-    <mergeCell ref="A11:L13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A7:F9" location="Instrument!A1" display="Instrument" xr:uid="{C4FE0A3F-D662-4BD4-A640-BC0CC046C1DF}"/>
@@ -17452,17 +17452,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="218" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="224" t="s">
         <v>532</v>
       </c>
-      <c r="C2" s="216"/>
+      <c r="C2" s="224"/>
       <c r="D2" s="136"/>
     </row>
     <row r="3" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="211"/>
+      <c r="A3" s="219"/>
       <c r="B3" s="43" t="s">
         <v>0</v>
       </c>
@@ -17474,7 +17474,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="211"/>
+      <c r="A4" s="219"/>
       <c r="B4" s="43" t="s">
         <v>1</v>
       </c>
@@ -17486,7 +17486,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="211"/>
+      <c r="A5" s="219"/>
       <c r="B5" s="43" t="s">
         <v>2</v>
       </c>
@@ -17498,7 +17498,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="211"/>
+      <c r="A6" s="219"/>
       <c r="B6" s="43" t="s">
         <v>3</v>
       </c>
@@ -17510,7 +17510,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="211"/>
+      <c r="A7" s="219"/>
       <c r="B7" s="43" t="s">
         <v>4</v>
       </c>
@@ -17522,7 +17522,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="211"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="43" t="s">
         <v>5</v>
       </c>
@@ -17534,7 +17534,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="211"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="43" t="s">
         <v>6</v>
       </c>
@@ -17546,7 +17546,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="211"/>
+      <c r="A10" s="219"/>
       <c r="B10" s="43" t="s">
         <v>7</v>
       </c>
@@ -17558,7 +17558,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="211"/>
+      <c r="A11" s="219"/>
       <c r="B11" s="43" t="s">
         <v>8</v>
       </c>
@@ -17570,7 +17570,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="211"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="43" t="s">
         <v>9</v>
       </c>
@@ -17582,7 +17582,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="211"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="43" t="s">
         <v>170</v>
       </c>
@@ -17594,7 +17594,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="211"/>
+      <c r="A14" s="219"/>
       <c r="B14" s="43" t="s">
         <v>10</v>
       </c>
@@ -17606,7 +17606,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="211"/>
+      <c r="A15" s="219"/>
       <c r="B15" s="43" t="s">
         <v>11</v>
       </c>
@@ -17618,7 +17618,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="211"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="43" t="s">
         <v>175</v>
       </c>
@@ -17630,7 +17630,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="211"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="43" t="s">
         <v>13</v>
       </c>
@@ -17642,7 +17642,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="211"/>
+      <c r="A18" s="219"/>
       <c r="B18" s="43" t="s">
         <v>14</v>
       </c>
@@ -17654,7 +17654,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="211"/>
+      <c r="A19" s="219"/>
       <c r="B19" s="43" t="s">
         <v>15</v>
       </c>
@@ -17666,7 +17666,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="211"/>
+      <c r="A20" s="219"/>
       <c r="B20" s="43" t="s">
         <v>16</v>
       </c>
@@ -17678,7 +17678,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="211"/>
+      <c r="A21" s="219"/>
       <c r="B21" s="43" t="s">
         <v>17</v>
       </c>
@@ -17690,7 +17690,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="211"/>
+      <c r="A22" s="219"/>
       <c r="B22" s="43" t="s">
         <v>18</v>
       </c>
@@ -17702,7 +17702,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="212"/>
+      <c r="A23" s="220"/>
       <c r="B23" s="44" t="s">
         <v>19</v>
       </c>
@@ -17720,17 +17720,17 @@
       <c r="D25" s="130"/>
     </row>
     <row r="26" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="207" t="s">
+      <c r="A26" s="215" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="217" t="s">
+      <c r="B26" s="225" t="s">
         <v>554</v>
       </c>
-      <c r="C26" s="217"/>
+      <c r="C26" s="225"/>
       <c r="D26" s="137"/>
     </row>
     <row r="27" spans="1:5" s="17" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="208"/>
+      <c r="A27" s="216"/>
       <c r="B27" s="43" t="s">
         <v>186</v>
       </c>
@@ -17743,7 +17743,7 @@
       <c r="E27"/>
     </row>
     <row r="28" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="208"/>
+      <c r="A28" s="216"/>
       <c r="B28" s="43" t="s">
         <v>0</v>
       </c>
@@ -17756,7 +17756,7 @@
       <c r="E28"/>
     </row>
     <row r="29" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="208"/>
+      <c r="A29" s="216"/>
       <c r="B29" s="43" t="s">
         <v>24</v>
       </c>
@@ -17769,7 +17769,7 @@
       <c r="E29"/>
     </row>
     <row r="30" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="208"/>
+      <c r="A30" s="216"/>
       <c r="B30" s="43" t="s">
         <v>190</v>
       </c>
@@ -17782,7 +17782,7 @@
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="208"/>
+      <c r="A31" s="216"/>
       <c r="B31" s="43" t="s">
         <v>2</v>
       </c>
@@ -17795,7 +17795,7 @@
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="208"/>
+      <c r="A32" s="216"/>
       <c r="B32" s="43" t="s">
         <v>3</v>
       </c>
@@ -17808,7 +17808,7 @@
       <c r="E32"/>
     </row>
     <row r="33" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="208"/>
+      <c r="A33" s="216"/>
       <c r="B33" s="43" t="s">
         <v>26</v>
       </c>
@@ -17821,7 +17821,7 @@
       <c r="E33"/>
     </row>
     <row r="34" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="208"/>
+      <c r="A34" s="216"/>
       <c r="B34" s="43" t="s">
         <v>27</v>
       </c>
@@ -17834,7 +17834,7 @@
       <c r="E34"/>
     </row>
     <row r="35" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="208"/>
+      <c r="A35" s="216"/>
       <c r="B35" s="43" t="s">
         <v>28</v>
       </c>
@@ -17847,7 +17847,7 @@
       <c r="E35"/>
     </row>
     <row r="36" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="208"/>
+      <c r="A36" s="216"/>
       <c r="B36" s="43" t="s">
         <v>7</v>
       </c>
@@ -17860,7 +17860,7 @@
       <c r="E36"/>
     </row>
     <row r="37" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="208"/>
+      <c r="A37" s="216"/>
       <c r="B37" s="43" t="s">
         <v>30</v>
       </c>
@@ -17873,7 +17873,7 @@
       <c r="E37"/>
     </row>
     <row r="38" spans="1:10" s="18" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="208"/>
+      <c r="A38" s="216"/>
       <c r="B38" s="43" t="s">
         <v>31</v>
       </c>
@@ -17886,7 +17886,7 @@
       <c r="E38"/>
     </row>
     <row r="39" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="208"/>
+      <c r="A39" s="216"/>
       <c r="B39" s="43" t="s">
         <v>14</v>
       </c>
@@ -17899,7 +17899,7 @@
       <c r="E39"/>
     </row>
     <row r="40" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="208"/>
+      <c r="A40" s="216"/>
       <c r="B40" s="43" t="s">
         <v>29</v>
       </c>
@@ -17912,7 +17912,7 @@
       <c r="E40"/>
     </row>
     <row r="41" spans="1:10" s="18" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="208"/>
+      <c r="A41" s="216"/>
       <c r="B41" s="43" t="s">
         <v>18</v>
       </c>
@@ -17925,7 +17925,7 @@
       <c r="E41"/>
     </row>
     <row r="42" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="208"/>
+      <c r="A42" s="216"/>
       <c r="B42" s="43" t="s">
         <v>32</v>
       </c>
@@ -17938,7 +17938,7 @@
       <c r="E42"/>
     </row>
     <row r="43" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="208"/>
+      <c r="A43" s="216"/>
       <c r="B43" s="43" t="s">
         <v>33</v>
       </c>
@@ -17951,7 +17951,7 @@
       <c r="E43"/>
     </row>
     <row r="44" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="208"/>
+      <c r="A44" s="216"/>
       <c r="B44" s="43" t="s">
         <v>34</v>
       </c>
@@ -17968,7 +17968,7 @@
       <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="208"/>
+      <c r="A45" s="216"/>
       <c r="B45" s="43" t="s">
         <v>35</v>
       </c>
@@ -17981,7 +17981,7 @@
       <c r="E45"/>
     </row>
     <row r="46" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="208"/>
+      <c r="A46" s="216"/>
       <c r="B46" s="43" t="s">
         <v>36</v>
       </c>
@@ -17994,7 +17994,7 @@
       <c r="E46"/>
     </row>
     <row r="47" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="208"/>
+      <c r="A47" s="216"/>
       <c r="B47" s="43" t="s">
         <v>37</v>
       </c>
@@ -18007,7 +18007,7 @@
       <c r="E47"/>
     </row>
     <row r="48" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="208"/>
+      <c r="A48" s="216"/>
       <c r="B48" s="43" t="s">
         <v>38</v>
       </c>
@@ -18020,7 +18020,7 @@
       <c r="E48"/>
     </row>
     <row r="49" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="209"/>
+      <c r="A49" s="217"/>
       <c r="B49" s="44" t="s">
         <v>19</v>
       </c>
@@ -18043,18 +18043,18 @@
       <c r="E51"/>
     </row>
     <row r="52" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="213" t="s">
+      <c r="A52" s="221" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="218" t="s">
+      <c r="B52" s="226" t="s">
         <v>577</v>
       </c>
-      <c r="C52" s="218"/>
+      <c r="C52" s="226"/>
       <c r="D52" s="138"/>
       <c r="E52"/>
     </row>
     <row r="53" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="214"/>
+      <c r="A53" s="222"/>
       <c r="B53" s="43" t="s">
         <v>54</v>
       </c>
@@ -18068,7 +18068,7 @@
       <c r="F53" s="131"/>
     </row>
     <row r="54" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="214"/>
+      <c r="A54" s="222"/>
       <c r="B54" s="43" t="s">
         <v>1</v>
       </c>
@@ -18082,7 +18082,7 @@
       <c r="F54" s="131"/>
     </row>
     <row r="55" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="214"/>
+      <c r="A55" s="222"/>
       <c r="B55" s="43" t="s">
         <v>2</v>
       </c>
@@ -18096,7 +18096,7 @@
       <c r="F55" s="131"/>
     </row>
     <row r="56" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="214"/>
+      <c r="A56" s="222"/>
       <c r="B56" s="43" t="s">
         <v>0</v>
       </c>
@@ -18110,7 +18110,7 @@
       <c r="F56" s="131"/>
     </row>
     <row r="57" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="214"/>
+      <c r="A57" s="222"/>
       <c r="B57" s="43" t="s">
         <v>3</v>
       </c>
@@ -18124,7 +18124,7 @@
       <c r="F57" s="131"/>
     </row>
     <row r="58" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="214"/>
+      <c r="A58" s="222"/>
       <c r="B58" s="43" t="s">
         <v>4</v>
       </c>
@@ -18138,7 +18138,7 @@
       <c r="F58" s="131"/>
     </row>
     <row r="59" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="214"/>
+      <c r="A59" s="222"/>
       <c r="B59" s="43" t="s">
         <v>7</v>
       </c>
@@ -18152,7 +18152,7 @@
       <c r="F59" s="131"/>
     </row>
     <row r="60" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="214"/>
+      <c r="A60" s="222"/>
       <c r="B60" s="43" t="s">
         <v>31</v>
       </c>
@@ -18166,7 +18166,7 @@
       <c r="F60" s="131"/>
     </row>
     <row r="61" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="214"/>
+      <c r="A61" s="222"/>
       <c r="B61" s="43" t="s">
         <v>55</v>
       </c>
@@ -18180,7 +18180,7 @@
       <c r="F61" s="131"/>
     </row>
     <row r="62" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="214"/>
+      <c r="A62" s="222"/>
       <c r="B62" s="43" t="s">
         <v>29</v>
       </c>
@@ -18194,7 +18194,7 @@
       <c r="F62" s="131"/>
     </row>
     <row r="63" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="214"/>
+      <c r="A63" s="222"/>
       <c r="B63" s="43" t="s">
         <v>30</v>
       </c>
@@ -18208,7 +18208,7 @@
       <c r="F63" s="131"/>
     </row>
     <row r="64" spans="1:10" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="214"/>
+      <c r="A64" s="222"/>
       <c r="B64" s="43" t="s">
         <v>18</v>
       </c>
@@ -18222,7 +18222,7 @@
       <c r="F64" s="131"/>
     </row>
     <row r="65" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="214"/>
+      <c r="A65" s="222"/>
       <c r="B65" s="43" t="s">
         <v>32</v>
       </c>
@@ -18236,7 +18236,7 @@
       <c r="F65" s="131"/>
     </row>
     <row r="66" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="214"/>
+      <c r="A66" s="222"/>
       <c r="B66" s="43" t="s">
         <v>33</v>
       </c>
@@ -18250,7 +18250,7 @@
       <c r="F66" s="131"/>
     </row>
     <row r="67" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="214"/>
+      <c r="A67" s="222"/>
       <c r="B67" s="43" t="s">
         <v>34</v>
       </c>
@@ -18264,7 +18264,7 @@
       <c r="F67" s="131"/>
     </row>
     <row r="68" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="214"/>
+      <c r="A68" s="222"/>
       <c r="B68" s="43" t="s">
         <v>35</v>
       </c>
@@ -18278,7 +18278,7 @@
       <c r="F68" s="131"/>
     </row>
     <row r="69" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="214"/>
+      <c r="A69" s="222"/>
       <c r="B69" s="43" t="s">
         <v>36</v>
       </c>
@@ -18292,7 +18292,7 @@
       <c r="F69" s="131"/>
     </row>
     <row r="70" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="214"/>
+      <c r="A70" s="222"/>
       <c r="B70" s="43" t="s">
         <v>37</v>
       </c>
@@ -18306,7 +18306,7 @@
       <c r="F70" s="131"/>
     </row>
     <row r="71" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="214"/>
+      <c r="A71" s="222"/>
       <c r="B71" s="43" t="s">
         <v>38</v>
       </c>
@@ -18320,7 +18320,7 @@
       <c r="F71" s="131"/>
     </row>
     <row r="72" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="215"/>
+      <c r="A72" s="223"/>
       <c r="B72" s="44" t="s">
         <v>19</v>
       </c>
@@ -18350,7 +18350,7 @@
       <c r="F74" s="131"/>
     </row>
     <row r="75" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="219" t="s">
+      <c r="A75" s="211" t="s">
         <v>224</v>
       </c>
       <c r="B75" s="235" t="s">
@@ -18362,7 +18362,7 @@
       <c r="F75" s="131"/>
     </row>
     <row r="76" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="220"/>
+      <c r="A76" s="212"/>
       <c r="B76" s="43" t="s">
         <v>70</v>
       </c>
@@ -18375,7 +18375,7 @@
       <c r="F76" s="131"/>
     </row>
     <row r="77" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="220"/>
+      <c r="A77" s="212"/>
       <c r="B77" s="43" t="s">
         <v>3</v>
       </c>
@@ -18387,7 +18387,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="220"/>
+      <c r="A78" s="212"/>
       <c r="B78" s="43" t="s">
         <v>71</v>
       </c>
@@ -18399,7 +18399,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="220"/>
+      <c r="A79" s="212"/>
       <c r="B79" s="43" t="s">
         <v>72</v>
       </c>
@@ -18411,7 +18411,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="220"/>
+      <c r="A80" s="212"/>
       <c r="B80" s="43" t="s">
         <v>7</v>
       </c>
@@ -18423,7 +18423,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" s="114" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="220"/>
+      <c r="A81" s="212"/>
       <c r="B81" s="43" t="s">
         <v>73</v>
       </c>
@@ -18435,7 +18435,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="220"/>
+      <c r="A82" s="212"/>
       <c r="B82" s="43" t="s">
         <v>29</v>
       </c>
@@ -18447,7 +18447,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="221"/>
+      <c r="A83" s="213"/>
       <c r="B83" s="44" t="s">
         <v>19</v>
       </c>
@@ -18460,17 +18460,17 @@
     </row>
     <row r="84" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="86" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="222" t="s">
+      <c r="A86" s="207" t="s">
         <v>142</v>
       </c>
-      <c r="B86" s="226" t="s">
+      <c r="B86" s="210" t="s">
         <v>595</v>
       </c>
-      <c r="C86" s="226"/>
+      <c r="C86" s="210"/>
       <c r="D86" s="140"/>
     </row>
     <row r="87" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="223"/>
+      <c r="A87" s="208"/>
       <c r="B87" s="43" t="s">
         <v>25</v>
       </c>
@@ -18482,7 +18482,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="223"/>
+      <c r="A88" s="208"/>
       <c r="B88" s="43" t="s">
         <v>2</v>
       </c>
@@ -18494,7 +18494,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="223"/>
+      <c r="A89" s="208"/>
       <c r="B89" s="43" t="s">
         <v>80</v>
       </c>
@@ -18506,7 +18506,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="223"/>
+      <c r="A90" s="208"/>
       <c r="B90" s="43" t="s">
         <v>100</v>
       </c>
@@ -18518,7 +18518,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="223"/>
+      <c r="A91" s="208"/>
       <c r="B91" s="43" t="s">
         <v>101</v>
       </c>
@@ -18530,7 +18530,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="223"/>
+      <c r="A92" s="208"/>
       <c r="B92" s="43" t="s">
         <v>91</v>
       </c>
@@ -18542,7 +18542,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="223"/>
+      <c r="A93" s="208"/>
       <c r="B93" s="43" t="s">
         <v>72</v>
       </c>
@@ -18554,7 +18554,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="223"/>
+      <c r="A94" s="208"/>
       <c r="B94" s="43" t="s">
         <v>102</v>
       </c>
@@ -18566,7 +18566,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="223"/>
+      <c r="A95" s="208"/>
       <c r="B95" s="43" t="s">
         <v>104</v>
       </c>
@@ -18578,7 +18578,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="223"/>
+      <c r="A96" s="208"/>
       <c r="B96" s="43" t="s">
         <v>103</v>
       </c>
@@ -18590,7 +18590,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="223"/>
+      <c r="A97" s="208"/>
       <c r="B97" s="43" t="s">
         <v>30</v>
       </c>
@@ -18602,7 +18602,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="223"/>
+      <c r="A98" s="208"/>
       <c r="B98" s="43" t="s">
         <v>105</v>
       </c>
@@ -18614,7 +18614,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="223"/>
+      <c r="A99" s="208"/>
       <c r="B99" s="43" t="s">
         <v>246</v>
       </c>
@@ -18626,7 +18626,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="223"/>
+      <c r="A100" s="208"/>
       <c r="B100" s="43" t="s">
         <v>248</v>
       </c>
@@ -18638,7 +18638,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="223"/>
+      <c r="A101" s="208"/>
       <c r="B101" s="43" t="s">
         <v>108</v>
       </c>
@@ -18650,7 +18650,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="223"/>
+      <c r="A102" s="208"/>
       <c r="B102" s="43" t="s">
         <v>109</v>
       </c>
@@ -18662,7 +18662,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="223"/>
+      <c r="A103" s="208"/>
       <c r="B103" s="43" t="s">
         <v>110</v>
       </c>
@@ -18674,7 +18674,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="224"/>
+      <c r="A104" s="209"/>
       <c r="B104" s="44" t="s">
         <v>19</v>
       </c>
@@ -18686,17 +18686,17 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="222" t="s">
+      <c r="A107" s="207" t="s">
         <v>141</v>
       </c>
-      <c r="B107" s="226" t="s">
+      <c r="B107" s="210" t="s">
         <v>612</v>
       </c>
-      <c r="C107" s="226"/>
+      <c r="C107" s="210"/>
       <c r="D107" s="140"/>
     </row>
     <row r="108" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="223"/>
+      <c r="A108" s="208"/>
       <c r="B108" s="43" t="s">
         <v>1</v>
       </c>
@@ -18708,7 +18708,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="223"/>
+      <c r="A109" s="208"/>
       <c r="B109" s="43" t="s">
         <v>80</v>
       </c>
@@ -18720,7 +18720,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="223"/>
+      <c r="A110" s="208"/>
       <c r="B110" s="43" t="s">
         <v>86</v>
       </c>
@@ -18732,7 +18732,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="223"/>
+      <c r="A111" s="208"/>
       <c r="B111" s="43" t="s">
         <v>87</v>
       </c>
@@ -18744,7 +18744,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="223"/>
+      <c r="A112" s="208"/>
       <c r="B112" s="43" t="s">
         <v>88</v>
       </c>
@@ -18756,7 +18756,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="223"/>
+      <c r="A113" s="208"/>
       <c r="B113" s="43" t="s">
         <v>7</v>
       </c>
@@ -18768,7 +18768,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="223"/>
+      <c r="A114" s="208"/>
       <c r="B114" s="43" t="s">
         <v>89</v>
       </c>
@@ -18780,7 +18780,7 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="223"/>
+      <c r="A115" s="208"/>
       <c r="B115" s="43" t="s">
         <v>90</v>
       </c>
@@ -18792,7 +18792,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="223"/>
+      <c r="A116" s="208"/>
       <c r="B116" s="43" t="s">
         <v>71</v>
       </c>
@@ -18805,7 +18805,7 @@
       <c r="E116" s="135"/>
     </row>
     <row r="117" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="223"/>
+      <c r="A117" s="208"/>
       <c r="B117" s="43" t="s">
         <v>91</v>
       </c>
@@ -18818,7 +18818,7 @@
       <c r="E117" s="135"/>
     </row>
     <row r="118" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="224"/>
+      <c r="A118" s="209"/>
       <c r="B118" s="44" t="s">
         <v>19</v>
       </c>
@@ -18830,17 +18830,17 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="222" t="s">
+      <c r="A121" s="207" t="s">
         <v>144</v>
       </c>
-      <c r="B121" s="226" t="s">
+      <c r="B121" s="210" t="s">
         <v>623</v>
       </c>
-      <c r="C121" s="226"/>
+      <c r="C121" s="210"/>
       <c r="D121" s="140"/>
     </row>
     <row r="122" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="223"/>
+      <c r="A122" s="208"/>
       <c r="B122" s="43" t="s">
         <v>24</v>
       </c>
@@ -18852,7 +18852,7 @@
       </c>
     </row>
     <row r="123" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="223"/>
+      <c r="A123" s="208"/>
       <c r="B123" s="43" t="s">
         <v>80</v>
       </c>
@@ -18864,7 +18864,7 @@
       </c>
     </row>
     <row r="124" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="223"/>
+      <c r="A124" s="208"/>
       <c r="B124" s="43" t="s">
         <v>74</v>
       </c>
@@ -18876,7 +18876,7 @@
       </c>
     </row>
     <row r="125" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="223"/>
+      <c r="A125" s="208"/>
       <c r="B125" s="43" t="s">
         <v>75</v>
       </c>
@@ -18888,7 +18888,7 @@
       </c>
     </row>
     <row r="126" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="223"/>
+      <c r="A126" s="208"/>
       <c r="B126" s="43" t="s">
         <v>77</v>
       </c>
@@ -18900,7 +18900,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="223"/>
+      <c r="A127" s="208"/>
       <c r="B127" s="43" t="s">
         <v>270</v>
       </c>
@@ -18912,7 +18912,7 @@
       </c>
     </row>
     <row r="128" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="224"/>
+      <c r="A128" s="209"/>
       <c r="B128" s="44" t="s">
         <v>19</v>
       </c>
@@ -18924,17 +18924,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="222" t="s">
+      <c r="A131" s="207" t="s">
         <v>138</v>
       </c>
-      <c r="B131" s="226" t="s">
+      <c r="B131" s="210" t="s">
         <v>631</v>
       </c>
-      <c r="C131" s="226"/>
+      <c r="C131" s="210"/>
       <c r="D131" s="140"/>
     </row>
     <row r="132" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="223"/>
+      <c r="A132" s="208"/>
       <c r="B132" s="43" t="s">
         <v>2</v>
       </c>
@@ -18946,7 +18946,7 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="223"/>
+      <c r="A133" s="208"/>
       <c r="B133" s="43" t="s">
         <v>80</v>
       </c>
@@ -18958,7 +18958,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="223"/>
+      <c r="A134" s="208"/>
       <c r="B134" s="43" t="s">
         <v>115</v>
       </c>
@@ -18970,7 +18970,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="223"/>
+      <c r="A135" s="208"/>
       <c r="B135" s="43" t="s">
         <v>276</v>
       </c>
@@ -18982,7 +18982,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="223"/>
+      <c r="A136" s="208"/>
       <c r="B136" s="43" t="s">
         <v>116</v>
       </c>
@@ -18994,7 +18994,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="223"/>
+      <c r="A137" s="208"/>
       <c r="B137" s="43" t="s">
         <v>7</v>
       </c>
@@ -19006,7 +19006,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="224"/>
+      <c r="A138" s="209"/>
       <c r="B138" s="44" t="s">
         <v>19</v>
       </c>
@@ -19024,17 +19024,17 @@
       <c r="C140" s="112"/>
     </row>
     <row r="141" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="222" t="s">
+      <c r="A141" s="207" t="s">
         <v>146</v>
       </c>
-      <c r="B141" s="226" t="s">
+      <c r="B141" s="210" t="s">
         <v>638</v>
       </c>
-      <c r="C141" s="226"/>
+      <c r="C141" s="210"/>
       <c r="D141" s="140"/>
     </row>
     <row r="142" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="223"/>
+      <c r="A142" s="208"/>
       <c r="B142" s="43" t="s">
         <v>3</v>
       </c>
@@ -19046,7 +19046,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="223"/>
+      <c r="A143" s="208"/>
       <c r="B143" s="43" t="s">
         <v>74</v>
       </c>
@@ -19058,7 +19058,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="223"/>
+      <c r="A144" s="208"/>
       <c r="B144" s="43" t="s">
         <v>75</v>
       </c>
@@ -19070,7 +19070,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="223"/>
+      <c r="A145" s="208"/>
       <c r="B145" s="43" t="s">
         <v>284</v>
       </c>
@@ -19082,7 +19082,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="223"/>
+      <c r="A146" s="208"/>
       <c r="B146" s="43" t="s">
         <v>77</v>
       </c>
@@ -19094,7 +19094,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="224"/>
+      <c r="A147" s="209"/>
       <c r="B147" s="44" t="s">
         <v>19</v>
       </c>
@@ -19106,17 +19106,17 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="222" t="s">
+      <c r="A150" s="207" t="s">
         <v>139</v>
       </c>
-      <c r="B150" s="226" t="s">
+      <c r="B150" s="210" t="s">
         <v>641</v>
       </c>
-      <c r="C150" s="226"/>
+      <c r="C150" s="210"/>
       <c r="D150" s="140"/>
     </row>
     <row r="151" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="223"/>
+      <c r="A151" s="208"/>
       <c r="B151" s="43" t="s">
         <v>71</v>
       </c>
@@ -19128,7 +19128,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="223"/>
+      <c r="A152" s="208"/>
       <c r="B152" s="43" t="s">
         <v>80</v>
       </c>
@@ -19140,7 +19140,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="223"/>
+      <c r="A153" s="208"/>
       <c r="B153" s="43" t="s">
         <v>126</v>
       </c>
@@ -19152,7 +19152,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="223"/>
+      <c r="A154" s="208"/>
       <c r="B154" s="43" t="s">
         <v>7</v>
       </c>
@@ -19164,7 +19164,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="223"/>
+      <c r="A155" s="208"/>
       <c r="B155" s="43" t="s">
         <v>127</v>
       </c>
@@ -19176,7 +19176,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="223"/>
+      <c r="A156" s="208"/>
       <c r="B156" s="43" t="s">
         <v>91</v>
       </c>
@@ -19188,7 +19188,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="224"/>
+      <c r="A157" s="209"/>
       <c r="B157" s="44" t="s">
         <v>19</v>
       </c>
@@ -19201,13 +19201,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A141:A147"/>
-    <mergeCell ref="A75:A83"/>
-    <mergeCell ref="A86:A104"/>
-    <mergeCell ref="A107:A118"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="A52:A72"/>
     <mergeCell ref="B141:C141"/>
     <mergeCell ref="A150:A157"/>
     <mergeCell ref="B150:C150"/>
@@ -19221,6 +19214,13 @@
     <mergeCell ref="B131:C131"/>
     <mergeCell ref="A121:A128"/>
     <mergeCell ref="A131:A138"/>
+    <mergeCell ref="A141:A147"/>
+    <mergeCell ref="A75:A83"/>
+    <mergeCell ref="A86:A104"/>
+    <mergeCell ref="A107:A118"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="A52:A72"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B90" r:id="rId1" display="https://semver.org/" xr:uid="{C97FB9E7-DF4B-4C76-B335-B7B92AA7CACE}"/>
@@ -20708,7 +20708,7 @@
   </sheetPr>
   <dimension ref="A1:V867"/>
   <sheetViews>
-    <sheetView topLeftCell="A855" zoomScaleNormal="100" zoomScaleSheetLayoutView="396" workbookViewId="0">
+    <sheetView topLeftCell="A843" zoomScaleNormal="100" zoomScaleSheetLayoutView="396" workbookViewId="0">
       <selection activeCell="A870" sqref="A870"/>
     </sheetView>
   </sheetViews>
@@ -42764,19 +42764,19 @@
     </row>
     <row r="2" spans="1:6" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C2" s="117" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>825</v>
+      </c>
+      <c r="E2" s="92" t="s">
         <v>804</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>827</v>
-      </c>
-      <c r="E2" s="92" t="s">
-        <v>806</v>
       </c>
       <c r="F2" s="115" t="s">
         <v>79</v>
@@ -42784,7 +42784,7 @@
     </row>
     <row r="3" spans="1:6" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="117"/>
@@ -42792,26 +42792,26 @@
     </row>
     <row r="4" spans="1:6" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B4" s="32"/>
       <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:6" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B5" s="32"/>
     </row>
     <row r="6" spans="1:6" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="91" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B7" s="32"/>
     </row>
@@ -43079,19 +43079,19 @@
     </row>
     <row r="3" spans="1:7" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>795</v>
       </c>
       <c r="D3" s="116" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="F3" s="35">
         <v>44284</v>
@@ -43319,10 +43319,10 @@
     </row>
     <row r="2" spans="1:11" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B2" s="72" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C2" s="72" t="s">
         <v>92</v>
@@ -43348,10 +43348,10 @@
     </row>
     <row r="3" spans="1:11" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="76" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B3" s="76" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C3" s="76" t="s">
         <v>96</v>
@@ -43377,10 +43377,10 @@
     </row>
     <row r="4" spans="1:11" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="89" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>98</v>
@@ -43478,7 +43478,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="22.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -43557,13 +43557,13 @@
     </row>
     <row r="2" spans="1:18" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="151" t="s">
-        <v>801</v>
+        <v>832</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C2" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D2" s="150" t="s">
         <v>787</v>
@@ -43578,7 +43578,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="K2" s="32" t="s">
         <v>112</v>
@@ -43595,13 +43595,13 @@
     </row>
     <row r="3" spans="1:18" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="151" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D3" s="150" t="s">
         <v>788</v>
@@ -43616,7 +43616,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="K3" s="32" t="s">
         <v>112</v>
@@ -43633,13 +43633,13 @@
     </row>
     <row r="4" spans="1:18" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="151" t="s">
-        <v>800</v>
+        <v>833</v>
       </c>
       <c r="B4" s="93" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D4" s="150" t="s">
         <v>789</v>
@@ -43654,7 +43654,7 @@
         <v>50</v>
       </c>
       <c r="I4" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="K4" s="32" t="s">
         <v>112</v>
@@ -43671,13 +43671,13 @@
     </row>
     <row r="5" spans="1:18" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="151" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B5" s="93" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D5" s="150" t="s">
         <v>790</v>
@@ -43692,7 +43692,7 @@
         <v>50</v>
       </c>
       <c r="I5" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="L5" s="32" t="s">
         <v>780</v>
@@ -43709,10 +43709,10 @@
         <v>797</v>
       </c>
       <c r="B6" s="93" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C6" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D6" s="150" t="s">
         <v>791</v>
@@ -43727,7 +43727,7 @@
         <v>50</v>
       </c>
       <c r="I6" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>781</v>
@@ -43744,10 +43744,10 @@
         <v>798</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C7" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D7" s="150" t="s">
         <v>792</v>
@@ -43762,7 +43762,7 @@
         <v>50</v>
       </c>
       <c r="I7" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>782</v>
@@ -43779,10 +43779,10 @@
         <v>799</v>
       </c>
       <c r="B8" s="93" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C8" s="93" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D8" s="150" t="s">
         <v>793</v>
@@ -43797,7 +43797,7 @@
         <v>50</v>
       </c>
       <c r="I8" s="88" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>783</v>
@@ -44028,16 +44028,16 @@
     </row>
     <row r="4" spans="1:7" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="93" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B4" s="93" t="s">
+        <v>809</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>811</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>813</v>
-      </c>
       <c r="D4" s="148" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E4" s="94"/>
       <c r="F4" s="32" t="s">
@@ -44072,6 +44072,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="f1a7acc2-f81a-433d-9c39-7b5f43052363">
+      <UserInfo>
+        <DisplayName>Lawrence Chiang</DisplayName>
+        <AccountId>82</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B573754F895C24CA1E5512CFED99DB0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f4855c6dd736ff9aff3ebd96dd4df84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49f006a8-6189-4577-95fd-d12e97e560aa" xmlns:ns3="f1a7acc2-f81a-433d-9c39-7b5f43052363" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fe0d94444280dde9da62946e52046e10" ns2:_="" ns3:_="">
     <xsd:import namespace="49f006a8-6189-4577-95fd-d12e97e560aa"/>
@@ -44282,30 +44305,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="f1a7acc2-f81a-433d-9c39-7b5f43052363">
-      <UserInfo>
-        <DisplayName>Lawrence Chiang</DisplayName>
-        <AccountId>82</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D8F596A-8119-441E-8E72-3B8F82046F19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78F5240-8910-4EAB-A5A8-13C69138C2A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f1a7acc2-f81a-433d-9c39-7b5f43052363"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72A0E3F5-9064-4AA8-9C48-1B983BD0AB22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44322,22 +44340,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78F5240-8910-4EAB-A5A8-13C69138C2A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f1a7acc2-f81a-433d-9c39-7b5f43052363"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D8F596A-8119-441E-8E72-3B8F82046F19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>